<commit_message>
Added profile need to test and upload to live.
</commit_message>
<xml_diff>
--- a/config/excel/data.xlsx
+++ b/config/excel/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Medication Treatment January 2021</t>
   </si>
@@ -100,7 +100,7 @@
     <t>Is Away:</t>
   </si>
   <si>
-    <t>Time Submitted:</t>
+    <t>Date Submitted:</t>
   </si>
   <si>
     <t>Given By:</t>
@@ -109,52 +109,49 @@
     <t>Notes:</t>
   </si>
   <si>
+    <t>Medication #2</t>
+  </si>
+  <si>
+    <t>3242424</t>
+  </si>
+  <si>
+    <t>Benzoid</t>
+  </si>
+  <si>
+    <t>Dr. Boid</t>
+  </si>
+  <si>
+    <t>3232342424</t>
+  </si>
+  <si>
+    <t>3 pills</t>
+  </si>
+  <si>
+    <t>For headaches</t>
+  </si>
+  <si>
     <t>1/18/2021</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>6:36 am</t>
+    <t>Take when needed.</t>
+  </si>
+  <si>
+    <t>01-18-2021</t>
+  </si>
+  <si>
+    <t>1/1/2021</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>1/19/2021 6:18 am</t>
   </si>
   <si>
     <t>Christopher McCoy</t>
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Medication #2</t>
-  </si>
-  <si>
-    <t>3242424</t>
-  </si>
-  <si>
-    <t>Benzoid</t>
-  </si>
-  <si>
-    <t>Dr. Boid</t>
-  </si>
-  <si>
-    <t>3232342424</t>
-  </si>
-  <si>
-    <t>3 pills</t>
-  </si>
-  <si>
-    <t>For headaches</t>
-  </si>
-  <si>
-    <t>Take when needed.</t>
-  </si>
-  <si>
-    <t>01-18-2021</t>
-  </si>
-  <si>
-    <t>6:30 am</t>
-  </si>
-  <si>
-    <t>Hes far far away</t>
   </si>
 </sst>
 </file>
@@ -208,7 +205,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -349,132 +346,115 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="0" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="0" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="0" t="s">
+      <c r="D32" s="0" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="E32" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Frontend took med works!
</commit_message>
<xml_diff>
--- a/config/excel/data.xlsx
+++ b/config/excel/data.xlsx
@@ -103,13 +103,13 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>6/10/2021</t>
+    <t>6/11/2021</t>
   </si>
   <si>
     <t>false</t>
   </si>
   <si>
-    <t>6/10/2021 @ 10:50 am</t>
+    <t>6/11/2021 @ 6:13 am</t>
   </si>
   <si>
     <t>John Snow</t>

</xml_diff>

<commit_message>
Export data works need to make sure the counters are right!
</commit_message>
<xml_diff>
--- a/config/excel/data.xlsx
+++ b/config/excel/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Medication Treatment June 2021</t>
   </si>
@@ -43,13 +43,13 @@
     <t>Rxs Number:</t>
   </si>
   <si>
-    <t/>
+    <t>-</t>
   </si>
   <si>
     <t>Name:</t>
   </si>
   <si>
-    <t>Benzoid 1</t>
+    <t>Benzoid</t>
   </si>
   <si>
     <t>Doctor's Name:</t>
@@ -61,7 +61,7 @@
     <t>Doctor's Contact:</t>
   </si>
   <si>
-    <t>9999999999</t>
+    <t>0000000000</t>
   </si>
   <si>
     <t>Dosage:</t>
@@ -79,31 +79,37 @@
     <t>Date Prescribed:</t>
   </si>
   <si>
-    <t>6/12/2021</t>
+    <t>06/05/2021</t>
   </si>
   <si>
     <t>Intructions:</t>
   </si>
   <si>
-    <t>Lets gooooooooo</t>
-  </si>
-  <si>
     <t>End Date:</t>
   </si>
   <si>
+    <t>06/22/2021</t>
+  </si>
+  <si>
     <t>Dates Taken:</t>
   </si>
   <si>
-    <t>Is Away:</t>
-  </si>
-  <si>
-    <t>Date Submitted:</t>
+    <t>Time:</t>
   </si>
   <si>
     <t>Given By:</t>
   </si>
   <si>
-    <t>Notes:</t>
+    <t>06/21/2021</t>
+  </si>
+  <si>
+    <t>12:14 pm</t>
+  </si>
+  <si>
+    <t>Admin One</t>
+  </si>
+  <si>
+    <t>12:15 pm</t>
   </si>
 </sst>
 </file>
@@ -157,7 +163,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -270,18 +276,18 @@
         <v>23</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -291,11 +297,27 @@
       <c r="C18" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="0" t="s">
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="B19" s="0" t="s">
         <v>30</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>